<commit_message>
code refactoring and big corrs matrix
</commit_message>
<xml_diff>
--- a/data/novelty/official/human_ratings/autdata_official_ratings_compiled_cleaned.xlsx
+++ b/data/novelty/official/human_ratings/autdata_official_ratings_compiled_cleaned.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\data\official\human_ratings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\data\novelty\official\human_ratings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21AF73E-F546-44DA-BB95-F7783B9511D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF573905-E0CE-48A2-BAB3-E1625610F0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1845" windowWidth="21495" windowHeight="11655" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23100" yWindow="4185" windowWidth="21495" windowHeight="11490" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10249" uniqueCount="2445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10249" uniqueCount="2444">
   <si>
     <t>id</t>
   </si>
@@ -7204,15 +7204,6 @@
     <t>resting objects</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>ratings</t>
-  </si>
-  <si>
-    <t>creativity</t>
-  </si>
-  <si>
     <t>use the tip as a screwdriver</t>
   </si>
   <si>
@@ -7373,6 +7364,12 @@
   </si>
   <si>
     <t>stack on top of each other</t>
+  </si>
+  <si>
+    <t>novelty_1</t>
+  </si>
+  <si>
+    <t>novelty_2</t>
   </si>
 </sst>
 </file>
@@ -7799,8 +7796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E383"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7813,16 +7810,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7867,7 +7864,7 @@
         <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>2423</v>
+        <v>2420</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -8394,7 +8391,7 @@
         <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>2439</v>
+        <v>2436</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -8768,7 +8765,7 @@
         <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>2421</v>
+        <v>2418</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -11114,7 +11111,7 @@
         <v>92</v>
       </c>
       <c r="C195" t="s">
-        <v>2422</v>
+        <v>2419</v>
       </c>
       <c r="D195">
         <v>4</v>
@@ -11964,7 +11961,7 @@
         <v>92</v>
       </c>
       <c r="C245" t="s">
-        <v>2418</v>
+        <v>2415</v>
       </c>
       <c r="D245">
         <v>3</v>
@@ -12032,7 +12029,7 @@
         <v>92</v>
       </c>
       <c r="C249" t="s">
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="D249">
         <v>1</v>
@@ -12389,7 +12386,7 @@
         <v>92</v>
       </c>
       <c r="C270" t="s">
-        <v>2420</v>
+        <v>2417</v>
       </c>
       <c r="D270">
         <v>3</v>
@@ -13579,7 +13576,7 @@
         <v>92</v>
       </c>
       <c r="C340" t="s">
-        <v>2391</v>
+        <v>2388</v>
       </c>
       <c r="D340">
         <v>3</v>
@@ -14328,8 +14325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E395"/>
   <sheetViews>
-    <sheetView topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="C337" sqref="C337"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14342,16 +14339,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -14787,7 +14784,7 @@
         <v>378</v>
       </c>
       <c r="C27" t="s">
-        <v>2405</v>
+        <v>2402</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -15093,7 +15090,7 @@
         <v>378</v>
       </c>
       <c r="C45" t="s">
-        <v>2403</v>
+        <v>2400</v>
       </c>
       <c r="D45">
         <v>4</v>
@@ -15654,7 +15651,7 @@
         <v>378</v>
       </c>
       <c r="C78" t="s">
-        <v>2400</v>
+        <v>2397</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -16130,7 +16127,7 @@
         <v>378</v>
       </c>
       <c r="C106" t="s">
-        <v>2401</v>
+        <v>2398</v>
       </c>
       <c r="D106">
         <v>4</v>
@@ -19683,7 +19680,7 @@
         <v>378</v>
       </c>
       <c r="C315" t="s">
-        <v>2402</v>
+        <v>2399</v>
       </c>
       <c r="D315">
         <v>3</v>
@@ -20040,7 +20037,7 @@
         <v>378</v>
       </c>
       <c r="C336" t="s">
-        <v>2436</v>
+        <v>2433</v>
       </c>
       <c r="D336">
         <v>2</v>
@@ -20295,7 +20292,7 @@
         <v>378</v>
       </c>
       <c r="C351" t="s">
-        <v>2404</v>
+        <v>2401</v>
       </c>
       <c r="D351">
         <v>4</v>
@@ -21061,8 +21058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E449"/>
   <sheetViews>
-    <sheetView topLeftCell="A426" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C441" sqref="C441"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21075,16 +21072,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -22948,7 +22945,7 @@
         <v>661</v>
       </c>
       <c r="C111" t="s">
-        <v>2394</v>
+        <v>2391</v>
       </c>
       <c r="D111">
         <v>2</v>
@@ -22965,7 +22962,7 @@
         <v>661</v>
       </c>
       <c r="C112" t="s">
-        <v>2397</v>
+        <v>2394</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -23713,7 +23710,7 @@
         <v>661</v>
       </c>
       <c r="C156" t="s">
-        <v>2393</v>
+        <v>2390</v>
       </c>
       <c r="D156">
         <v>5</v>
@@ -24869,7 +24866,7 @@
         <v>661</v>
       </c>
       <c r="C224" t="s">
-        <v>2398</v>
+        <v>2395</v>
       </c>
       <c r="D224">
         <v>2</v>
@@ -24886,7 +24883,7 @@
         <v>661</v>
       </c>
       <c r="C225" t="s">
-        <v>2395</v>
+        <v>2392</v>
       </c>
       <c r="D225">
         <v>2</v>
@@ -26178,7 +26175,7 @@
         <v>661</v>
       </c>
       <c r="C301" t="s">
-        <v>2396</v>
+        <v>2393</v>
       </c>
       <c r="D301">
         <v>2</v>
@@ -28507,7 +28504,7 @@
         <v>661</v>
       </c>
       <c r="C438" t="s">
-        <v>2399</v>
+        <v>2396</v>
       </c>
       <c r="D438">
         <v>3</v>
@@ -28712,8 +28709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E479"/>
   <sheetViews>
-    <sheetView topLeftCell="A414" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C427" sqref="C427"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28726,16 +28723,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -29426,7 +29423,7 @@
         <v>1002</v>
       </c>
       <c r="C42" t="s">
-        <v>2428</v>
+        <v>2425</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -30684,7 +30681,7 @@
         <v>1002</v>
       </c>
       <c r="C116" t="s">
-        <v>2426</v>
+        <v>2423</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -31925,7 +31922,7 @@
         <v>1002</v>
       </c>
       <c r="C189" t="s">
-        <v>2429</v>
+        <v>2426</v>
       </c>
       <c r="D189">
         <v>2</v>
@@ -32384,7 +32381,7 @@
         <v>1002</v>
       </c>
       <c r="C216" t="s">
-        <v>2425</v>
+        <v>2422</v>
       </c>
       <c r="D216">
         <v>2</v>
@@ -32554,7 +32551,7 @@
         <v>1002</v>
       </c>
       <c r="C226" t="s">
-        <v>2427</v>
+        <v>2424</v>
       </c>
       <c r="D226">
         <v>3</v>
@@ -34424,7 +34421,7 @@
         <v>1002</v>
       </c>
       <c r="C336" t="s">
-        <v>2430</v>
+        <v>2427</v>
       </c>
       <c r="D336">
         <v>2</v>
@@ -36873,8 +36870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="H232" sqref="H232"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36887,16 +36884,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -38811,7 +38808,7 @@
         <v>1338</v>
       </c>
       <c r="C114" t="s">
-        <v>2435</v>
+        <v>2432</v>
       </c>
       <c r="D114">
         <v>5</v>
@@ -38845,7 +38842,7 @@
         <v>1338</v>
       </c>
       <c r="C116" t="s">
-        <v>2441</v>
+        <v>2438</v>
       </c>
       <c r="D116">
         <v>4</v>
@@ -39525,7 +39522,7 @@
         <v>1338</v>
       </c>
       <c r="C156" t="s">
-        <v>2432</v>
+        <v>2429</v>
       </c>
       <c r="D156">
         <v>3</v>
@@ -39593,7 +39590,7 @@
         <v>1338</v>
       </c>
       <c r="C160" t="s">
-        <v>2433</v>
+        <v>2430</v>
       </c>
       <c r="D160">
         <v>3</v>
@@ -40868,7 +40865,7 @@
         <v>1338</v>
       </c>
       <c r="C235" t="s">
-        <v>2442</v>
+        <v>2439</v>
       </c>
       <c r="D235">
         <v>2</v>
@@ -41990,7 +41987,7 @@
         <v>1338</v>
       </c>
       <c r="C301" t="s">
-        <v>2434</v>
+        <v>2431</v>
       </c>
       <c r="D301">
         <v>3</v>
@@ -42041,7 +42038,7 @@
         <v>1338</v>
       </c>
       <c r="C304" t="s">
-        <v>2431</v>
+        <v>2428</v>
       </c>
       <c r="D304">
         <v>2</v>
@@ -43810,8 +43807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E422"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="H288" sqref="H288"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43824,16 +43821,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -45697,7 +45694,7 @@
         <v>1610</v>
       </c>
       <c r="C111" t="s">
-        <v>2424</v>
+        <v>2421</v>
       </c>
       <c r="D111">
         <v>4</v>
@@ -48672,7 +48669,7 @@
         <v>1610</v>
       </c>
       <c r="C286" t="s">
-        <v>2440</v>
+        <v>2437</v>
       </c>
       <c r="D286">
         <v>4</v>
@@ -51002,8 +50999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E443"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51016,16 +51013,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2389</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -53025,7 +53022,7 @@
         <v>1862</v>
       </c>
       <c r="C119" t="s">
-        <v>2437</v>
+        <v>2434</v>
       </c>
       <c r="D119">
         <v>4</v>
@@ -53518,7 +53515,7 @@
         <v>1862</v>
       </c>
       <c r="C148" t="s">
-        <v>2438</v>
+        <v>2435</v>
       </c>
       <c r="D148">
         <v>3</v>
@@ -54062,7 +54059,7 @@
         <v>1862</v>
       </c>
       <c r="C180" t="s">
-        <v>2411</v>
+        <v>2408</v>
       </c>
       <c r="D180">
         <v>3</v>
@@ -54113,7 +54110,7 @@
         <v>1862</v>
       </c>
       <c r="C183" t="s">
-        <v>2410</v>
+        <v>2407</v>
       </c>
       <c r="D183">
         <v>4</v>
@@ -54538,7 +54535,7 @@
         <v>1862</v>
       </c>
       <c r="C208" t="s">
-        <v>2412</v>
+        <v>2409</v>
       </c>
       <c r="D208">
         <v>3</v>
@@ -55099,7 +55096,7 @@
         <v>1862</v>
       </c>
       <c r="C241" t="s">
-        <v>2413</v>
+        <v>2410</v>
       </c>
       <c r="D241">
         <v>2</v>
@@ -55405,7 +55402,7 @@
         <v>1862</v>
       </c>
       <c r="C259" t="s">
-        <v>2415</v>
+        <v>2412</v>
       </c>
       <c r="D259">
         <v>2</v>
@@ -55813,7 +55810,7 @@
         <v>1862</v>
       </c>
       <c r="C283" t="s">
-        <v>2417</v>
+        <v>2414</v>
       </c>
       <c r="D283">
         <v>2</v>
@@ -57547,7 +57544,7 @@
         <v>1862</v>
       </c>
       <c r="C385" t="s">
-        <v>2414</v>
+        <v>2411</v>
       </c>
       <c r="D385">
         <v>3</v>
@@ -57768,7 +57765,7 @@
         <v>1862</v>
       </c>
       <c r="C398" t="s">
-        <v>2416</v>
+        <v>2413</v>
       </c>
       <c r="D398">
         <v>3</v>
@@ -58551,8 +58548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="H341" sqref="H341"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58565,16 +58562,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2388</v>
+        <v>2442</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2390</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -61305,7 +61302,7 @@
         <v>2163</v>
       </c>
       <c r="C162" t="s">
-        <v>2409</v>
+        <v>2406</v>
       </c>
       <c r="D162">
         <v>3</v>
@@ -62478,7 +62475,7 @@
         <v>2163</v>
       </c>
       <c r="C231" t="s">
-        <v>2443</v>
+        <v>2440</v>
       </c>
       <c r="D231">
         <v>2</v>
@@ -62512,7 +62509,7 @@
         <v>2163</v>
       </c>
       <c r="C233" t="s">
-        <v>2407</v>
+        <v>2404</v>
       </c>
       <c r="D233">
         <v>2</v>
@@ -63515,7 +63512,7 @@
         <v>2163</v>
       </c>
       <c r="C292" t="s">
-        <v>2408</v>
+        <v>2405</v>
       </c>
       <c r="D292">
         <v>2</v>
@@ -64314,7 +64311,7 @@
         <v>2163</v>
       </c>
       <c r="C339" t="s">
-        <v>2444</v>
+        <v>2441</v>
       </c>
       <c r="D339">
         <v>2</v>
@@ -65113,7 +65110,7 @@
         <v>2163</v>
       </c>
       <c r="C386" t="s">
-        <v>2406</v>
+        <v>2403</v>
       </c>
       <c r="D386">
         <v>2</v>

</xml_diff>